<commit_message>
Modificacion 2 de estudio de fact tecnica
</commit_message>
<xml_diff>
--- a/Estudio de factibilida POLO360.xlsx
+++ b/Estudio de factibilida POLO360.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64a0d8c99e961e89/Escritorio/Proyecto 2/Proyecto2_G2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_A5C01EAAB5CAAAD5DF723847337DA67E2BA48162" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4110E3A0-2D00-4BDC-8CD5-88BA12821A89}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_A5C01EAAB5CAAAD5DF723847337DA67E2BA48162" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54322078-A7D9-4761-85FD-ED947BAEB4E7}"/>
   <bookViews>
     <workbookView xWindow="2655" yWindow="1140" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,13 +200,13 @@
     <t>Herramienta de diseño grafico</t>
   </si>
   <si>
-    <t>Amazon Web Services</t>
-  </si>
-  <si>
     <t>Servicio de host para el sitio web</t>
   </si>
   <si>
     <t xml:space="preserve">Conclusión: Según los recursos técnicos que se requieren para el desarrollo del proyecto, estos se pueden conseguir en el país, por tal razón, el proyecto es factible técnicamente </t>
+  </si>
+  <si>
+    <t>Hosting 506</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;₡&quot;* #,##0.00_-;\-&quot;₡&quot;* #,##0.00_-;_-&quot;₡&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +324,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -699,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -771,63 +784,63 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -851,6 +864,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,346 +1098,346 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="29" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="29" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="33">
+      <c r="C4" s="28"/>
+      <c r="D4" s="35">
         <f>(3*5*12)*4000</f>
         <v>720000</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="33">
+      <c r="E4" s="28"/>
+      <c r="F4" s="35">
         <f>D4</f>
         <v>720000</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27">
+      <c r="C5" s="31"/>
+      <c r="D5" s="41">
         <f>(3*5*12)*3000</f>
         <v>540000</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27">
+      <c r="E5" s="31"/>
+      <c r="F5" s="41">
         <f>D5*2</f>
         <v>1080000</v>
       </c>
-      <c r="G5" s="40"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27">
+      <c r="C6" s="31"/>
+      <c r="D6" s="41">
         <f>D4</f>
         <v>720000</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27">
+      <c r="E6" s="31"/>
+      <c r="F6" s="41">
         <f>D6</f>
         <v>720000</v>
       </c>
-      <c r="G6" s="40"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="41" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="42">
+      <c r="E7" s="28"/>
+      <c r="F7" s="43">
         <f>SUM(F4:G6)</f>
         <v>2520000</v>
       </c>
-      <c r="G7" s="40"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="40"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="40"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="29" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="31"/>
+      <c r="E10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="33">
+      <c r="D11" s="28"/>
+      <c r="E11" s="35">
         <v>300</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="6">
         <f>E11*140</f>
         <v>42000</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="36">
         <v>1</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="7">
         <f>15*600</f>
         <v>9000</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="40"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="31"/>
+      <c r="E14" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
+      <c r="A15" s="33">
         <v>1</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="31"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="8">
         <f>200*600</f>
         <v>120000</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="29" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="26"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="9">
         <f>G11+G12+G15</f>
         <v>171000</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="40"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="29" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="29" t="s">
+      <c r="D18" s="31"/>
+      <c r="E18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="26"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="30">
+      <c r="A19" s="33">
         <v>1</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="33">
+      <c r="D19" s="28"/>
+      <c r="E19" s="35">
         <v>1500</v>
       </c>
-      <c r="F19" s="31"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="6">
         <f>E19</f>
         <v>1500</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="34">
+      <c r="A20" s="36">
         <v>2</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27">
+      <c r="D20" s="31"/>
+      <c r="E20" s="41">
         <v>10000</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="7">
         <f t="shared" ref="G20:G22" si="0">E20*A20</f>
         <v>20000</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30">
+      <c r="A21" s="33">
         <f>10*12</f>
         <v>120</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="33">
+      <c r="D21" s="28"/>
+      <c r="E21" s="35">
         <v>300</v>
       </c>
-      <c r="F21" s="31"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
         <v>36000</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34">
+      <c r="A22" s="36">
         <f>60*4</f>
         <v>240</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="25" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27">
+      <c r="D22" s="31"/>
+      <c r="E22" s="41">
         <v>5000</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="7">
         <f t="shared" si="0"/>
         <v>1200000</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="35" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="9">
         <f>SUM(G19:G22)</f>
         <v>1257500</v>
@@ -1431,54 +1448,54 @@
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="46"/>
       <c r="G24" s="11">
         <f>SUM(G23,G16,F7)</f>
         <v>3948500</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="40"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="29" t="s">
+      <c r="B26" s="31"/>
+      <c r="C26" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="29" t="s">
+      <c r="D26" s="31"/>
+      <c r="E26" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="26"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30">
+      <c r="A27" s="33">
         <v>1</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="31"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="6">
         <f>G24*0.1</f>
         <v>394850</v>
@@ -1486,25 +1503,25 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="40"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="46"/>
       <c r="G30" s="12">
         <f>G24+G27</f>
         <v>4343350</v>
@@ -1512,71 +1529,71 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="40"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="29" t="s">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="29" t="s">
+      <c r="D33" s="31"/>
+      <c r="E33" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30">
+      <c r="A34" s="33">
         <v>1</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="31"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="6">
         <f>100*600</f>
         <v>60000</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30">
+      <c r="A35" s="33">
         <v>1</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="31"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="6">
         <f>120*600</f>
         <v>72000</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="13">
         <f>SUM(G34:G35)</f>
         <v>132000</v>
@@ -2548,38 +2565,30 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="B5:C5"/>
@@ -2589,13 +2598,30 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="A25:G25"/>
@@ -2606,23 +2632,14 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -2631,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1001"/>
+  <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2646,7 +2663,7 @@
     <col min="5" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
         <v>33</v>
       </c>
@@ -2655,7 +2672,7 @@
       <c r="D1" s="58"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>34</v>
       </c>
@@ -2670,7 +2687,7 @@
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>36</v>
       </c>
@@ -2685,7 +2702,7 @@
       </c>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="60"/>
       <c r="C4" s="17" t="s">
@@ -2696,7 +2713,7 @@
       </c>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>40</v>
       </c>
@@ -2709,18 +2726,19 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
       <c r="B6" s="49"/>
       <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="61"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
         <v>10</v>
       </c>
@@ -2731,11 +2749,11 @@
         <v>43</v>
       </c>
       <c r="D7" s="19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="60"/>
       <c r="B8" s="60"/>
       <c r="C8" s="22" t="s">
@@ -2744,7 +2762,7 @@
       <c r="D8" s="48"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="60"/>
       <c r="B9" s="60"/>
       <c r="C9" s="22" t="s">
@@ -2753,7 +2771,7 @@
       <c r="D9" s="60"/>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="60"/>
       <c r="B10" s="49"/>
       <c r="C10" s="23" t="s">
@@ -2762,7 +2780,7 @@
       <c r="D10" s="49"/>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="18" t="s">
         <v>47</v>
@@ -2775,7 +2793,7 @@
       </c>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
         <v>16</v>
       </c>
@@ -2790,14 +2808,14 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="60"/>
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="60"/>
       <c r="B14" s="18" t="s">
         <v>51</v>
@@ -2810,7 +2828,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="60"/>
       <c r="B15" s="18" t="s">
         <v>53</v>
@@ -2822,8 +2840,9 @@
         <v>1</v>
       </c>
       <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="61"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="60"/>
       <c r="B16" s="21" t="s">
         <v>55</v>
@@ -2851,11 +2870,11 @@
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="D18" s="18">
         <v>1</v>
@@ -2864,7 +2883,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
@@ -3875,6 +3894,6 @@
     <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>